<commit_message>
Added translations for MYA to RefApp translation sheet.
</commit_message>
<xml_diff>
--- a/Source/rap/Documents/Internal/Localization/StringLocalization.xlsx
+++ b/Source/rap/Documents/Internal/Localization/StringLocalization.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philips/Documents/LocalizationScript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310274421/Development/plf-android/Source/rap/Documents/Internal/Localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33340" windowHeight="18160" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-11940" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4523" uniqueCount="3759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4558" uniqueCount="3793">
   <si>
     <t>Reference</t>
   </si>
@@ -34109,13 +34109,115 @@
   </si>
   <si>
     <t>Keys</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Moment_Text</t>
+  </si>
+  <si>
+    <t>I allow Philips to store my data in cloud</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Moment_Help</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Coaching_Text</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Coaching_Help</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Binary_Text</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Binary_Help</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Clickstream_Text</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_Clickstream_Help</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_ResearchAnalytics_Text</t>
+  </si>
+  <si>
+    <t>RA_MYA_Consent_ResearchAnalytics_Help</t>
+  </si>
+  <si>
+    <t>Giving this consent you are allowing Philips to store information related to you</t>
+  </si>
+  <si>
+    <t>I allow Philips to use my data for Coaching purposes</t>
+  </si>
+  <si>
+    <t>Giving this consent you are allowing Philips to process information related to you</t>
+  </si>
+  <si>
+    <t>I allow Philips to store binary data</t>
+  </si>
+  <si>
+    <t>I allow Philips to use my mobile application usage statistics</t>
+  </si>
+  <si>
+    <t>Giving this consent you are allowing Philips to process mobile usage statistics related to you</t>
+  </si>
+  <si>
+    <t>I allow Philips to use my data for Research and Analytics purposes</t>
+  </si>
+  <si>
+    <t>Research and Analytics purpose explanation</t>
+  </si>
+  <si>
+    <t>de-I allow Philips to store my data in cloud</t>
+  </si>
+  <si>
+    <t>de-Giving this consent you are allowing Philips to store information related to you</t>
+  </si>
+  <si>
+    <t>de-I allow Philips to store binary data</t>
+  </si>
+  <si>
+    <t>de-I allow Philips to use my mobile application usage statistics</t>
+  </si>
+  <si>
+    <t>de-Giving this consent you are allowing Philips to process mobile usage statistics related to you</t>
+  </si>
+  <si>
+    <t>de-I allow Philips to use my data for Research and Analytics purposes</t>
+  </si>
+  <si>
+    <t>de-Research and Analytics purpose explanation</t>
+  </si>
+  <si>
+    <t>fa-I allow Philips to store my data in cloud</t>
+  </si>
+  <si>
+    <t>fa-Giving this consent you are allowing Philips to store information related to you</t>
+  </si>
+  <si>
+    <t>fa-Giving this consent you are allowing Philips to process information related to you</t>
+  </si>
+  <si>
+    <t>fa-I allow Philips to store binary data</t>
+  </si>
+  <si>
+    <t>fa-I allow Philips to use my mobile application usage statistics</t>
+  </si>
+  <si>
+    <t>fa-Giving this consent you are allowing Philips to process mobile usage statistics related to you</t>
+  </si>
+  <si>
+    <t>fa-I allow Philips to use my data for Research and Analytics purposes</t>
+  </si>
+  <si>
+    <t>fa-Research and Analytics purpose explanation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -34234,6 +34336,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -34375,10 +34492,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -34519,8 +34638,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -34798,13 +34926,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:AZ22"/>
+    <sheetView tabSelected="1" topLeftCell="AE119" workbookViewId="0">
+      <selection activeCell="AQ124" sqref="AQ124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
@@ -49090,45 +49218,1611 @@
         <v>3754</v>
       </c>
     </row>
-    <row r="115" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" ht="126" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
+      <c r="C115" s="50" t="s">
+        <v>3759</v>
+      </c>
+      <c r="D115" s="50"/>
+      <c r="E115" s="51" t="s">
+        <v>3760</v>
+      </c>
+      <c r="F115" s="51" t="s">
+        <v>3778</v>
+      </c>
+      <c r="G115" s="51" t="s">
+        <v>3785</v>
+      </c>
+      <c r="H115" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E115)</f>
+        <v>zh-Hans-CN-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="I115" s="51" t="str">
+        <f>CONCATENATE(I4, "-", E115)</f>
+        <v>zh-Hant-TW-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="J115" s="51" t="str">
+        <f>CONCATENATE(J4, "-", E115)</f>
+        <v>zh-Hant-HK-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="K115" s="51" t="str">
+        <f>CONCATENATE(K4, "-", E115)</f>
+        <v>pt-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="L115" s="51" t="str">
+        <f>CONCATENATE(L4, "-", E115)</f>
+        <v>ru-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="M115" s="51" t="str">
+        <f>CONCATENATE(M4, "-", E115)</f>
+        <v>ar-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="N115" s="51" t="str">
+        <f>CONCATENATE(N4, "-", E115)</f>
+        <v>ja-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="O115" s="51" t="str">
+        <f>CONCATENATE(O4, "-", E115)</f>
+        <v>nl-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="P115" s="51" t="str">
+        <f>CONCATENATE(P4, "-", E115)</f>
+        <v>it-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="Q115" s="51" t="str">
+        <f>CONCATENATE(Q4, "-", E115)</f>
+        <v>pl-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="R115" s="51" t="str">
+        <f>CONCATENATE(R4, "-", E115)</f>
+        <v>es-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="S115" s="51" t="str">
+        <f>CONCATENATE(S4, "-", E115)</f>
+        <v>ko-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="T115" s="51" t="str">
+        <f>CONCATENATE(T4, "-", E115)</f>
+        <v>cs-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="U115" s="51" t="str">
+        <f>CONCATENATE(U4, "-", E115)</f>
+        <v>en-GB-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="V115" s="51" t="str">
+        <f>CONCATENATE(V4, "-", E115)</f>
+        <v>fr-CA-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="W115" s="51" t="str">
+        <f>CONCATENATE(W4, "-", E115)</f>
+        <v>ro-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="X115" s="51" t="str">
+        <f>CONCATENATE(X4, "-", E115)</f>
+        <v>es-MX-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="Y115" s="51" t="str">
+        <f>CONCATENATE(Y4, "-", E115)</f>
+        <v>nb-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="Z115" s="51" t="str">
+        <f>CONCATENATE(Z4, "-", E115)</f>
+        <v>bg-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AA115" s="51" t="str">
+        <f>CONCATENATE(AA4, "-", E115)</f>
+        <v>hr-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AB115" s="51" t="str">
+        <f>CONCATENATE(AB4, "-", E115)</f>
+        <v>et-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AC115" s="51" t="str">
+        <f>CONCATENATE(AC4, "-", E115)</f>
+        <v>el-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AD115" s="51" t="str">
+        <f>CONCATENATE(AD4, "-", E115)</f>
+        <v>he-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AE115" s="51" t="str">
+        <f>CONCATENATE(AE4, "-", E115)</f>
+        <v>hu-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AF115" s="51" t="str">
+        <f>CONCATENATE(AF4, "-", E115)</f>
+        <v>lv-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AG115" s="51" t="str">
+        <f>CONCATENATE(AG4, "-", E115)</f>
+        <v>lt-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AH115" s="51" t="str">
+        <f>CONCATENATE(AH4, "-", E115)</f>
+        <v>pt-BR-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AI115" s="51" t="str">
+        <f>CONCATENATE(AI4, "-", E115)</f>
+        <v>sk-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AJ115" s="51" t="str">
+        <f>CONCATENATE(AJ4, "-", E115)</f>
+        <v>sl-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AK115" s="51" t="str">
+        <f>CONCATENATE(AK4, "-", E115)</f>
+        <v>es-AR-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AL115" s="51" t="str">
+        <f>CONCATENATE(AL4, "-", E115)</f>
+        <v>th-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AM115" s="51" t="str">
+        <f>CONCATENATE(AM4, "-", E115)</f>
+        <v>vi-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AN115" s="51" t="str">
+        <f>CONCATENATE(AN4, "-", E115)</f>
+        <v>da-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AO115" s="51" t="str">
+        <f>CONCATENATE(AO4, "-", E115)</f>
+        <v>fi-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AP115" s="51" t="str">
+        <f>CONCATENATE(AP4, "-", E115)</f>
+        <v>sv-I allow Philips to store my data in cloud</v>
+      </c>
+      <c r="AQ115" s="51" t="str">
+        <f>CONCATENATE(AQ4, "-", E115)</f>
+        <v>tr-I allow Philips to store my data in cloud</v>
+      </c>
     </row>
-    <row r="116" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:43" ht="190" x14ac:dyDescent="0.25">
       <c r="A116" s="15"/>
       <c r="B116" s="15"/>
+      <c r="C116" s="50" t="s">
+        <v>3761</v>
+      </c>
+      <c r="E116" s="52" t="s">
+        <v>3770</v>
+      </c>
+      <c r="F116" s="52" t="str">
+        <f>CONCATENATE(F4, "-", E116)</f>
+        <v>de-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="G116" s="52" t="str">
+        <f>CONCATENATE(G4, "-", E116)</f>
+        <v>fr-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="H116" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E116)</f>
+        <v>zh-Hans-CN-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="I116" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E116)</f>
+        <v>zh-Hant-TW-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="J116" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E116)</f>
+        <v>zh-Hant-HK-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="K116" s="51" t="str">
+        <f>CONCATENATE(K4, "-", E116)</f>
+        <v>pt-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="L116" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E116)</f>
+        <v>ru-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="M116" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E116)</f>
+        <v>ar-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="N116" s="51" t="str">
+        <f>CONCATENATE(N4, "-", E116)</f>
+        <v>ja-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="O116" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E116)</f>
+        <v>nl-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="P116" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E116)</f>
+        <v>it-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="Q116" s="51" t="str">
+        <f>CONCATENATE(Q4, "-", E116)</f>
+        <v>pl-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="R116" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E116)</f>
+        <v>es-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="S116" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E116)</f>
+        <v>ko-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="T116" s="51" t="str">
+        <f>CONCATENATE(T4, "-", E116)</f>
+        <v>cs-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="U116" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E116)</f>
+        <v>en-GB-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="V116" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E116)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="W116" s="51" t="str">
+        <f>CONCATENATE(W4, "-", E116)</f>
+        <v>ro-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="X116" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E116)</f>
+        <v>es-MX-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="Y116" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E116)</f>
+        <v>nb-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="Z116" s="51" t="str">
+        <f>CONCATENATE(Z4, "-", E116)</f>
+        <v>bg-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AA116" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E116)</f>
+        <v>hr-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AB116" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E116)</f>
+        <v>et-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AC116" s="51" t="str">
+        <f>CONCATENATE(AC4, "-", E116)</f>
+        <v>el-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AD116" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E116)</f>
+        <v>he-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AE116" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E116)</f>
+        <v>hu-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AF116" s="51" t="str">
+        <f>CONCATENATE(AF4, "-", E116)</f>
+        <v>lv-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AG116" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E116)</f>
+        <v>lt-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AH116" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E116)</f>
+        <v>pt-BR-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AI116" s="51" t="str">
+        <f>CONCATENATE(AI4, "-", E116)</f>
+        <v>sk-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AJ116" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E116)</f>
+        <v>sl-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AK116" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E116)</f>
+        <v>es-AR-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AL116" s="51" t="str">
+        <f>CONCATENATE(AL4, "-", E116)</f>
+        <v>th-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AM116" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E116)</f>
+        <v>vi-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AN116" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E116)</f>
+        <v>da-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AO116" s="51" t="str">
+        <f>CONCATENATE(AO4, "-", E116)</f>
+        <v>fi-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AP116" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E116)</f>
+        <v>sv-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AQ116" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E116)</f>
+        <v>tr-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
     </row>
-    <row r="117" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:43" ht="114" x14ac:dyDescent="0.25">
       <c r="A117" s="36"/>
       <c r="B117" s="36"/>
+      <c r="C117" s="50" t="s">
+        <v>3762</v>
+      </c>
+      <c r="E117" s="52" t="s">
+        <v>3771</v>
+      </c>
+      <c r="F117" s="52" t="str">
+        <f>CONCATENATE(F4, "-", E117)</f>
+        <v>de-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="G117" s="52" t="str">
+        <f>CONCATENATE(G4, "-", E117)</f>
+        <v>fr-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="H117" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E117)</f>
+        <v>zh-Hans-CN-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="I117" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E117)</f>
+        <v>zh-Hant-TW-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="J117" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E117)</f>
+        <v>zh-Hant-HK-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="K117" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E117)</f>
+        <v>pt-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="L117" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E117)</f>
+        <v>ru-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="M117" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E117)</f>
+        <v>ar-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="N117" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E117)</f>
+        <v>ja-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="O117" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E117)</f>
+        <v>nl-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="P117" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E117)</f>
+        <v>it-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="Q117" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E117)</f>
+        <v>pl-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="R117" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E117)</f>
+        <v>es-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="S117" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E117)</f>
+        <v>ko-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="T117" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E117)</f>
+        <v>cs-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="U117" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E117)</f>
+        <v>en-GB-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="V117" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E117)</f>
+        <v>fr-CA-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="W117" s="52" t="str">
+        <f>CONCATENATE(W4, "-", E117)</f>
+        <v>ro-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="X117" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E117)</f>
+        <v>es-MX-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="Y117" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E117)</f>
+        <v>nb-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="Z117" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E117)</f>
+        <v>bg-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AA117" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E117)</f>
+        <v>hr-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AB117" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E117)</f>
+        <v>et-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AC117" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E117)</f>
+        <v>el-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AD117" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E117)</f>
+        <v>he-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AE117" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E117)</f>
+        <v>hu-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AF117" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E117)</f>
+        <v>lv-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AG117" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E117)</f>
+        <v>lt-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AH117" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E117)</f>
+        <v>pt-BR-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AI117" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E117)</f>
+        <v>sk-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AJ117" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E117)</f>
+        <v>sl-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AK117" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E117)</f>
+        <v>es-AR-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AL117" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E117)</f>
+        <v>th-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AM117" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E117)</f>
+        <v>vi-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AN117" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E117)</f>
+        <v>da-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AO117" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E117)</f>
+        <v>fi-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AP117" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E117)</f>
+        <v>sv-I allow Philips to use my data for Coaching purposes</v>
+      </c>
+      <c r="AQ117" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E117)</f>
+        <v>tr-I allow Philips to use my data for Coaching purposes</v>
+      </c>
     </row>
-    <row r="118" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:43" ht="190" x14ac:dyDescent="0.25">
       <c r="A118" s="36"/>
       <c r="B118" s="36"/>
+      <c r="C118" s="50" t="s">
+        <v>3763</v>
+      </c>
+      <c r="E118" s="52" t="s">
+        <v>3772</v>
+      </c>
+      <c r="F118" s="52" t="str">
+        <f>CONCATENATE(F4, "-", E118)</f>
+        <v>de-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="G118" s="52" t="s">
+        <v>3787</v>
+      </c>
+      <c r="H118" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E118)</f>
+        <v>zh-Hans-CN-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="I118" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E118)</f>
+        <v>zh-Hant-TW-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="J118" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E118)</f>
+        <v>zh-Hant-HK-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="K118" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E118)</f>
+        <v>pt-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="L118" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E118)</f>
+        <v>ru-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="M118" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E118)</f>
+        <v>ar-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="N118" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E118)</f>
+        <v>ja-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="O118" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E118)</f>
+        <v>nl-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="P118" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E118)</f>
+        <v>it-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="Q118" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E118)</f>
+        <v>pl-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="R118" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E118)</f>
+        <v>es-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="S118" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E118)</f>
+        <v>ko-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="T118" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E118)</f>
+        <v>cs-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="U118" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E118)</f>
+        <v>en-GB-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="V118" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E118)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="W118" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E118)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="X118" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E118)</f>
+        <v>es-MX-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="Y118" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E118)</f>
+        <v>nb-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="Z118" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E118)</f>
+        <v>bg-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AA118" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E118)</f>
+        <v>hr-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AB118" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E118)</f>
+        <v>et-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AC118" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E118)</f>
+        <v>el-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AD118" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E118)</f>
+        <v>he-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AE118" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E118)</f>
+        <v>hu-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AF118" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E118)</f>
+        <v>lv-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AG118" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E118)</f>
+        <v>lt-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AH118" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E118)</f>
+        <v>pt-BR-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AI118" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E118)</f>
+        <v>sk-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AJ118" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E118)</f>
+        <v>sl-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AK118" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E118)</f>
+        <v>es-AR-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AL118" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E118)</f>
+        <v>th-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AM118" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E118)</f>
+        <v>vi-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AN118" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E118)</f>
+        <v>da-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AO118" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E118)</f>
+        <v>fi-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AP118" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E118)</f>
+        <v>sv-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AQ118" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E118)</f>
+        <v>tr-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
     </row>
-    <row r="119" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:43" ht="95" x14ac:dyDescent="0.25">
       <c r="A119" s="36"/>
       <c r="B119" s="36"/>
+      <c r="C119" s="50" t="s">
+        <v>3764</v>
+      </c>
+      <c r="E119" s="52" t="s">
+        <v>3773</v>
+      </c>
+      <c r="F119" s="52" t="s">
+        <v>3780</v>
+      </c>
+      <c r="G119" s="52" t="s">
+        <v>3788</v>
+      </c>
+      <c r="H119" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E119)</f>
+        <v>zh-Hans-CN-I allow Philips to store binary data</v>
+      </c>
+      <c r="I119" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E119)</f>
+        <v>zh-Hant-TW-I allow Philips to store binary data</v>
+      </c>
+      <c r="J119" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E119)</f>
+        <v>zh-Hant-HK-I allow Philips to store binary data</v>
+      </c>
+      <c r="K119" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E119)</f>
+        <v>pt-I allow Philips to store binary data</v>
+      </c>
+      <c r="L119" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E119)</f>
+        <v>ru-I allow Philips to store binary data</v>
+      </c>
+      <c r="M119" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E119)</f>
+        <v>ar-I allow Philips to store binary data</v>
+      </c>
+      <c r="N119" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E118)</f>
+        <v>ja-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="O119" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E119)</f>
+        <v>nl-I allow Philips to store binary data</v>
+      </c>
+      <c r="P119" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E119)</f>
+        <v>it-I allow Philips to store binary data</v>
+      </c>
+      <c r="Q119" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E119)</f>
+        <v>pl-I allow Philips to store binary data</v>
+      </c>
+      <c r="R119" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E119)</f>
+        <v>es-I allow Philips to store binary data</v>
+      </c>
+      <c r="S119" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E119)</f>
+        <v>ko-I allow Philips to store binary data</v>
+      </c>
+      <c r="T119" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E119)</f>
+        <v>cs-I allow Philips to store binary data</v>
+      </c>
+      <c r="U119" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E119)</f>
+        <v>en-GB-I allow Philips to store binary data</v>
+      </c>
+      <c r="V119" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E119)</f>
+        <v>fr-CA-I allow Philips to store binary data</v>
+      </c>
+      <c r="W119" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E119)</f>
+        <v>fr-CA-I allow Philips to store binary data</v>
+      </c>
+      <c r="X119" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E119)</f>
+        <v>es-MX-I allow Philips to store binary data</v>
+      </c>
+      <c r="Y119" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E119)</f>
+        <v>nb-I allow Philips to store binary data</v>
+      </c>
+      <c r="Z119" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E119)</f>
+        <v>bg-I allow Philips to store binary data</v>
+      </c>
+      <c r="AA119" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E119)</f>
+        <v>hr-I allow Philips to store binary data</v>
+      </c>
+      <c r="AB119" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E119)</f>
+        <v>et-I allow Philips to store binary data</v>
+      </c>
+      <c r="AC119" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E119)</f>
+        <v>el-I allow Philips to store binary data</v>
+      </c>
+      <c r="AD119" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E119)</f>
+        <v>he-I allow Philips to store binary data</v>
+      </c>
+      <c r="AE119" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E119)</f>
+        <v>hu-I allow Philips to store binary data</v>
+      </c>
+      <c r="AF119" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E119)</f>
+        <v>lv-I allow Philips to store binary data</v>
+      </c>
+      <c r="AG119" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E119)</f>
+        <v>lt-I allow Philips to store binary data</v>
+      </c>
+      <c r="AH119" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E119)</f>
+        <v>pt-BR-I allow Philips to store binary data</v>
+      </c>
+      <c r="AI119" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E118)</f>
+        <v>sk-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AJ119" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E119)</f>
+        <v>sl-I allow Philips to store binary data</v>
+      </c>
+      <c r="AK119" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E119)</f>
+        <v>es-AR-I allow Philips to store binary data</v>
+      </c>
+      <c r="AL119" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E119)</f>
+        <v>th-I allow Philips to store binary data</v>
+      </c>
+      <c r="AM119" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E119)</f>
+        <v>vi-I allow Philips to store binary data</v>
+      </c>
+      <c r="AN119" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E119)</f>
+        <v>da-I allow Philips to store binary data</v>
+      </c>
+      <c r="AO119" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E119)</f>
+        <v>fi-I allow Philips to store binary data</v>
+      </c>
+      <c r="AP119" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E119)</f>
+        <v>sv-I allow Philips to store binary data</v>
+      </c>
+      <c r="AQ119" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E119)</f>
+        <v>tr-I allow Philips to store binary data</v>
+      </c>
     </row>
-    <row r="120" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:43" ht="190" x14ac:dyDescent="0.25">
       <c r="A120" s="15"/>
       <c r="B120" s="15"/>
+      <c r="C120" s="50" t="s">
+        <v>3765</v>
+      </c>
+      <c r="E120" s="52" t="s">
+        <v>3770</v>
+      </c>
+      <c r="F120" s="52" t="s">
+        <v>3779</v>
+      </c>
+      <c r="G120" s="52" t="s">
+        <v>3786</v>
+      </c>
+      <c r="H120" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E120)</f>
+        <v>zh-Hans-CN-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="I120" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E120)</f>
+        <v>zh-Hant-TW-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="J120" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E120)</f>
+        <v>zh-Hant-HK-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="K120" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E119)</f>
+        <v>pt-I allow Philips to store binary data</v>
+      </c>
+      <c r="L120" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E120)</f>
+        <v>ru-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="M120" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E120)</f>
+        <v>ar-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="N120" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E120)</f>
+        <v>ja-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="O120" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E120)</f>
+        <v>nl-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="P120" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E120)</f>
+        <v>it-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="Q120" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E120)</f>
+        <v>pl-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="R120" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E120)</f>
+        <v>es-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="S120" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E120)</f>
+        <v>ko-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="T120" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E120)</f>
+        <v>cs-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="U120" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E120)</f>
+        <v>en-GB-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="V120" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E120)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="W120" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E120)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="X120" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E120)</f>
+        <v>es-MX-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="Y120" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E120)</f>
+        <v>nb-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="Z120" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E120)</f>
+        <v>bg-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AA120" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E120)</f>
+        <v>hr-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AB120" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E120)</f>
+        <v>et-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AC120" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E120)</f>
+        <v>el-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AD120" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E120)</f>
+        <v>he-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AE120" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E120)</f>
+        <v>hu-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AF120" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E120)</f>
+        <v>lv-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AG120" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E120)</f>
+        <v>lt-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AH120" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E120)</f>
+        <v>pt-BR-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AI120" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E118)</f>
+        <v>sk-Giving this consent you are allowing Philips to process information related to you</v>
+      </c>
+      <c r="AJ120" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E120)</f>
+        <v>sl-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AK120" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E120)</f>
+        <v>es-AR-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AL120" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E120)</f>
+        <v>th-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AM120" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E119)</f>
+        <v>vi-I allow Philips to store binary data</v>
+      </c>
+      <c r="AN120" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E120)</f>
+        <v>da-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AO120" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E120)</f>
+        <v>fi-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AP120" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E120)</f>
+        <v>sv-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AQ120" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E120)</f>
+        <v>tr-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
     </row>
-    <row r="121" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:43" ht="95" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
       <c r="B121" s="15"/>
+      <c r="C121" s="50" t="s">
+        <v>3766</v>
+      </c>
+      <c r="E121" s="52" t="s">
+        <v>3774</v>
+      </c>
+      <c r="F121" s="52" t="s">
+        <v>3781</v>
+      </c>
+      <c r="G121" s="52" t="s">
+        <v>3789</v>
+      </c>
+      <c r="H121" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E121)</f>
+        <v>zh-Hans-CN-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="I121" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E121)</f>
+        <v>zh-Hant-TW-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="J121" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E121)</f>
+        <v>zh-Hant-HK-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="K121" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E121)</f>
+        <v>pt-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="L121" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E121)</f>
+        <v>ru-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="M121" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E121)</f>
+        <v>ar-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="N121" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E121)</f>
+        <v>ja-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="O121" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E121)</f>
+        <v>nl-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="P121" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E121)</f>
+        <v>it-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="Q121" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E121)</f>
+        <v>pl-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="R121" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E121)</f>
+        <v>es-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="S121" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E121)</f>
+        <v>ko-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="T121" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E121)</f>
+        <v>cs-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="U121" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E121)</f>
+        <v>en-GB-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="V121" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E121)</f>
+        <v>fr-CA-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="W121" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E121)</f>
+        <v>fr-CA-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="X121" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E121)</f>
+        <v>es-MX-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="Y121" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E1121)</f>
+        <v>nb-</v>
+      </c>
+      <c r="Z121" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E121)</f>
+        <v>bg-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AA121" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E121)</f>
+        <v>hr-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AB121" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E121)</f>
+        <v>et-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AC121" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E121)</f>
+        <v>el-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AD121" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E121)</f>
+        <v>he-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AE121" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E121)</f>
+        <v>hu-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AF121" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E121)</f>
+        <v>lv-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AG121" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E121)</f>
+        <v>lt-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AH121" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E121)</f>
+        <v>pt-BR-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AI121" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E121)</f>
+        <v>sk-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AJ121" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E121)</f>
+        <v>sl-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AK121" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E121)</f>
+        <v>es-AR-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AL121" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E121)</f>
+        <v>th-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AM121" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E120)</f>
+        <v>vi-Giving this consent you are allowing Philips to store information related to you</v>
+      </c>
+      <c r="AN121" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E121)</f>
+        <v>da-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AO121" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E121)</f>
+        <v>fi-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AP121" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E121)</f>
+        <v>sv-I allow Philips to use my mobile application usage statistics</v>
+      </c>
+      <c r="AQ121" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E121)</f>
+        <v>tr-I allow Philips to use my mobile application usage statistics</v>
+      </c>
     </row>
-    <row r="122" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:43" ht="228" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122" s="15"/>
+      <c r="C122" s="50" t="s">
+        <v>3767</v>
+      </c>
+      <c r="E122" s="52" t="s">
+        <v>3775</v>
+      </c>
+      <c r="F122" s="52" t="s">
+        <v>3782</v>
+      </c>
+      <c r="G122" s="52" t="s">
+        <v>3790</v>
+      </c>
+      <c r="H122" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E122)</f>
+        <v>zh-Hans-CN-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="I122" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E122)</f>
+        <v>zh-Hant-TW-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="J122" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E122)</f>
+        <v>zh-Hant-HK-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="K122" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E122)</f>
+        <v>pt-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="L122" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E122)</f>
+        <v>ru-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="M122" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E122)</f>
+        <v>ar-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="N122" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E122)</f>
+        <v>ja-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="O122" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E122)</f>
+        <v>nl-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="P122" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E122)</f>
+        <v>it-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="Q122" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E122)</f>
+        <v>pl-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="R122" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E122)</f>
+        <v>es-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="S122" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E122)</f>
+        <v>ko-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="T122" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E122)</f>
+        <v>cs-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="U122" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E122)</f>
+        <v>en-GB-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="V122" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E122)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="W122" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E122)</f>
+        <v>fr-CA-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="X122" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E122)</f>
+        <v>es-MX-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="Y122" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E122)</f>
+        <v>nb-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="Z122" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E122)</f>
+        <v>bg-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AA122" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E122)</f>
+        <v>hr-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AB122" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E122)</f>
+        <v>et-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AC122" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E122)</f>
+        <v>el-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AD122" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E122)</f>
+        <v>he-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AE122" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E122)</f>
+        <v>hu-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AF122" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E122)</f>
+        <v>lv-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AG122" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E122)</f>
+        <v>lt-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AH122" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E122)</f>
+        <v>pt-BR-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AI122" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E122)</f>
+        <v>sk-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AJ122" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E122)</f>
+        <v>sl-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AK122" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E122)</f>
+        <v>es-AR-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AL122" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E122)</f>
+        <v>th-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AM122" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E122)</f>
+        <v>vi-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AN122" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E122)</f>
+        <v>da-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AO122" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E122)</f>
+        <v>fi-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AP122" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E122)</f>
+        <v>sv-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
+      <c r="AQ122" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E122)</f>
+        <v>tr-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+      </c>
     </row>
-    <row r="123" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:43" ht="152" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123" s="15"/>
+      <c r="C123" s="50" t="s">
+        <v>3768</v>
+      </c>
+      <c r="E123" s="52" t="s">
+        <v>3776</v>
+      </c>
+      <c r="F123" s="52" t="s">
+        <v>3783</v>
+      </c>
+      <c r="G123" s="52" t="s">
+        <v>3791</v>
+      </c>
+      <c r="H123" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E123)</f>
+        <v>zh-Hans-CN-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="I123" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E123)</f>
+        <v>zh-Hant-TW-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="J123" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E123)</f>
+        <v>zh-Hant-HK-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="K123" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E123)</f>
+        <v>pt-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="L123" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E123)</f>
+        <v>ru-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="M123" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E123)</f>
+        <v>ar-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="N123" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E123)</f>
+        <v>ja-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="O123" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E123)</f>
+        <v>nl-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="P123" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E123)</f>
+        <v>it-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="Q123" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E123)</f>
+        <v>pl-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="R123" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E123)</f>
+        <v>es-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="S123" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E123)</f>
+        <v>ko-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="T123" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E123)</f>
+        <v>cs-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="U123" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E123)</f>
+        <v>en-GB-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="V123" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E123)</f>
+        <v>fr-CA-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="W123" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E123)</f>
+        <v>fr-CA-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="X123" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E123)</f>
+        <v>es-MX-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="Y123" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E123)</f>
+        <v>nb-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="Z123" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E123)</f>
+        <v>bg-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AA123" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E123)</f>
+        <v>hr-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AB123" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E123)</f>
+        <v>et-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AC123" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E123)</f>
+        <v>el-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AD123" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E123)</f>
+        <v>he-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AE123" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E123)</f>
+        <v>hu-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AF123" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E123)</f>
+        <v>lv-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AG123" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E123)</f>
+        <v>lt-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AH123" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E123)</f>
+        <v>pt-BR-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AI123" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E123)</f>
+        <v>sk-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AJ123" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E123)</f>
+        <v>sl-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AK123" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E123)</f>
+        <v>es-AR-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AL123" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E123)</f>
+        <v>th-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AM123" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E123)</f>
+        <v>vi-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AN123" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E123)</f>
+        <v>da-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AO123" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E123)</f>
+        <v>fi-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AP123" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E123)</f>
+        <v>sv-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
+      <c r="AQ123" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E123)</f>
+        <v>tr-I allow Philips to use my data for Research and Analytics purposes</v>
+      </c>
     </row>
-    <row r="124" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:43" ht="133" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124" s="15"/>
+      <c r="C124" s="50" t="s">
+        <v>3769</v>
+      </c>
+      <c r="E124" s="52" t="s">
+        <v>3777</v>
+      </c>
+      <c r="F124" s="52" t="s">
+        <v>3784</v>
+      </c>
+      <c r="G124" s="52" t="s">
+        <v>3792</v>
+      </c>
+      <c r="H124" s="51" t="str">
+        <f>CONCATENATE(H4, "-", E124)</f>
+        <v>zh-Hans-CN-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="I124" s="52" t="str">
+        <f>CONCATENATE(I4, "-", E124)</f>
+        <v>zh-Hant-TW-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="J124" s="52" t="str">
+        <f>CONCATENATE(J4, "-", E124)</f>
+        <v>zh-Hant-HK-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="K124" s="52" t="str">
+        <f>CONCATENATE(K4, "-", E124)</f>
+        <v>pt-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="L124" s="52" t="str">
+        <f>CONCATENATE(L4, "-", E124)</f>
+        <v>ru-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="M124" s="52" t="str">
+        <f>CONCATENATE(M4, "-", E124)</f>
+        <v>ar-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="N124" s="52" t="str">
+        <f>CONCATENATE(N4, "-", E124)</f>
+        <v>ja-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="O124" s="52" t="str">
+        <f>CONCATENATE(O4, "-", E124)</f>
+        <v>nl-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="P124" s="52" t="str">
+        <f>CONCATENATE(P4, "-", E124)</f>
+        <v>it-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="Q124" s="52" t="str">
+        <f>CONCATENATE(Q4, "-", E124)</f>
+        <v>pl-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="R124" s="52" t="str">
+        <f>CONCATENATE(R4, "-", E124)</f>
+        <v>es-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="S124" s="52" t="str">
+        <f>CONCATENATE(S4, "-", E124)</f>
+        <v>ko-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="T124" s="52" t="str">
+        <f>CONCATENATE(T4, "-", E124)</f>
+        <v>cs-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="U124" s="52" t="str">
+        <f>CONCATENATE(U4, "-", E124)</f>
+        <v>en-GB-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="V124" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E124)</f>
+        <v>fr-CA-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="W124" s="52" t="str">
+        <f>CONCATENATE(V4, "-", E124)</f>
+        <v>fr-CA-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="X124" s="52" t="str">
+        <f>CONCATENATE(X4, "-", E124)</f>
+        <v>es-MX-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="Y124" s="52" t="str">
+        <f>CONCATENATE(Y4, "-", E124)</f>
+        <v>nb-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="Z124" s="52" t="str">
+        <f>CONCATENATE(Z4, "-", E124)</f>
+        <v>bg-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AA124" s="52" t="str">
+        <f>CONCATENATE(AA4, "-", E124)</f>
+        <v>hr-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AB124" s="52" t="str">
+        <f>CONCATENATE(AB4, "-", E124)</f>
+        <v>et-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AC124" s="52" t="str">
+        <f>CONCATENATE(AC4, "-", E124)</f>
+        <v>el-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AD124" s="52" t="str">
+        <f>CONCATENATE(AD4, "-", E124)</f>
+        <v>he-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AE124" s="52" t="str">
+        <f>CONCATENATE(AE4, "-", E124)</f>
+        <v>hu-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AF124" s="52" t="str">
+        <f>CONCATENATE(AF4, "-", E124)</f>
+        <v>lv-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AG124" s="52" t="str">
+        <f>CONCATENATE(AG4, "-", E124)</f>
+        <v>lt-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AH124" s="52" t="str">
+        <f>CONCATENATE(AH4, "-", E124)</f>
+        <v>pt-BR-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AI124" s="52" t="str">
+        <f>CONCATENATE(AI4, "-", E124)</f>
+        <v>sk-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AJ124" s="52" t="str">
+        <f>CONCATENATE(AJ4, "-", E124)</f>
+        <v>sl-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AK124" s="52" t="str">
+        <f>CONCATENATE(AK4, "-", E124)</f>
+        <v>es-AR-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AL124" s="52" t="str">
+        <f>CONCATENATE(AL4, "-", E124)</f>
+        <v>th-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AM124" s="52" t="str">
+        <f>CONCATENATE(AM4, "-", E124)</f>
+        <v>vi-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AN124" s="52" t="str">
+        <f>CONCATENATE(AN4, "-", E124)</f>
+        <v>da-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AO124" s="52" t="str">
+        <f>CONCATENATE(AO4, "-", E124)</f>
+        <v>fi-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AP124" s="52" t="str">
+        <f>CONCATENATE(AP4, "-", E124)</f>
+        <v>sv-Research and Analytics purpose explanation</v>
+      </c>
+      <c r="AQ124" s="52" t="str">
+        <f>CONCATENATE(AQ4, "-", E124)</f>
+        <v>tr-Research and Analytics purpose explanation</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -49171,5 +50865,6 @@
     <hyperlink ref="E2" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#101107 Added marketing help text
</commit_message>
<xml_diff>
--- a/Source/rap/Documents/Internal/Localization/StringLocalization.xlsx
+++ b/Source/rap/Documents/Internal/Localization/StringLocalization.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310274421/Development/plf-android/Source/rap/Documents/Internal/Localization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310286027/dev/Apgrade/android/plf-android/Source/rap/Documents/Internal/Localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-11940" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4558" uniqueCount="3793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4560" uniqueCount="3795">
   <si>
     <t>Reference</t>
   </si>
@@ -34211,6 +34211,12 @@
   </si>
   <si>
     <t>fa-Research and Analytics purpose explanation</t>
+  </si>
+  <si>
+    <t>RA_MYA_Marketing_Help_Text</t>
+  </si>
+  <si>
+    <t>As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</t>
   </si>
 </sst>
 </file>
@@ -34497,7 +34503,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -34643,6 +34649,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -34924,10 +34933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ124"/>
+  <dimension ref="A1:AQ126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE119" workbookViewId="0">
-      <selection activeCell="AQ124" sqref="AQ124"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49218,7 +49227,7 @@
         <v>3754</v>
       </c>
     </row>
-    <row r="115" spans="1:43" ht="126" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" ht="90" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="50" t="s">
@@ -49780,8 +49789,8 @@
         <v>fr-CA-Giving this consent you are allowing Philips to process information related to you</v>
       </c>
       <c r="W118" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E118)</f>
-        <v>fr-CA-Giving this consent you are allowing Philips to process information related to you</v>
+        <f>CONCATENATE(W4, "-", E118)</f>
+        <v>ro-Giving this consent you are allowing Philips to process information related to you</v>
       </c>
       <c r="X118" s="52" t="str">
         <f>CONCATENATE(X4, "-", E118)</f>
@@ -49940,8 +49949,8 @@
         <v>fr-CA-I allow Philips to store binary data</v>
       </c>
       <c r="W119" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E119)</f>
-        <v>fr-CA-I allow Philips to store binary data</v>
+        <f>CONCATENATE(W4, "-", E119)</f>
+        <v>ro-I allow Philips to store binary data</v>
       </c>
       <c r="X119" s="52" t="str">
         <f>CONCATENATE(X4, "-", E119)</f>
@@ -50100,8 +50109,8 @@
         <v>fr-CA-Giving this consent you are allowing Philips to store information related to you</v>
       </c>
       <c r="W120" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E120)</f>
-        <v>fr-CA-Giving this consent you are allowing Philips to store information related to you</v>
+        <f>CONCATENATE(W4, "-", E120)</f>
+        <v>ro-Giving this consent you are allowing Philips to store information related to you</v>
       </c>
       <c r="X120" s="52" t="str">
         <f>CONCATENATE(X4, "-", E120)</f>
@@ -50260,8 +50269,8 @@
         <v>fr-CA-I allow Philips to use my mobile application usage statistics</v>
       </c>
       <c r="W121" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E121)</f>
-        <v>fr-CA-I allow Philips to use my mobile application usage statistics</v>
+        <f>CONCATENATE(W4, "-", E121)</f>
+        <v>ro-I allow Philips to use my mobile application usage statistics</v>
       </c>
       <c r="X121" s="52" t="str">
         <f>CONCATENATE(X4, "-", E121)</f>
@@ -50420,8 +50429,8 @@
         <v>fr-CA-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
       </c>
       <c r="W122" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E122)</f>
-        <v>fr-CA-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
+        <f>CONCATENATE(W4, "-", E122)</f>
+        <v>ro-Giving this consent you are allowing Philips to process mobile usage statistics related to you</v>
       </c>
       <c r="X122" s="52" t="str">
         <f>CONCATENATE(X4, "-", E122)</f>
@@ -50580,8 +50589,8 @@
         <v>fr-CA-I allow Philips to use my data for Research and Analytics purposes</v>
       </c>
       <c r="W123" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E123)</f>
-        <v>fr-CA-I allow Philips to use my data for Research and Analytics purposes</v>
+        <f>CONCATENATE(W4, "-", E123)</f>
+        <v>ro-I allow Philips to use my data for Research and Analytics purposes</v>
       </c>
       <c r="X123" s="52" t="str">
         <f>CONCATENATE(X4, "-", E123)</f>
@@ -50740,8 +50749,8 @@
         <v>fr-CA-Research and Analytics purpose explanation</v>
       </c>
       <c r="W124" s="52" t="str">
-        <f>CONCATENATE(V4, "-", E124)</f>
-        <v>fr-CA-Research and Analytics purpose explanation</v>
+        <f>CONCATENATE(W4, "-", E124)</f>
+        <v>ro-Research and Analytics purpose explanation</v>
       </c>
       <c r="X124" s="52" t="str">
         <f>CONCATENATE(X4, "-", E124)</f>
@@ -50823,6 +50832,169 @@
         <f>CONCATENATE(AQ4, "-", E124)</f>
         <v>tr-Research and Analytics purpose explanation</v>
       </c>
+    </row>
+    <row r="125" spans="1:43" ht="97" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C125" s="50" t="s">
+        <v>3793</v>
+      </c>
+      <c r="E125" s="53" t="s">
+        <v>3794</v>
+      </c>
+      <c r="F125" s="52" t="str">
+        <f t="shared" ref="F125:S125" si="0">CONCATENATE(F$4, "-",$E$125)</f>
+        <v>de-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="G125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>fr-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="H125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>zh-Hans-CN-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="I125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>zh-Hant-TW-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="J125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>zh-Hant-HK-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="K125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>pt-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="L125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>ru-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="M125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>ar-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="N125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>ja-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="O125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>nl-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="P125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>it-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="Q125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>pl-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="R125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>es-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="S125" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>ko-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="T125" s="52" t="str">
+        <f t="shared" ref="T125:V125" si="1">CONCATENATE(T$4, "-",$E$125)</f>
+        <v>cs-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="U125" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>en-GB-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="V125" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>fr-CA-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="W125" s="52" t="str">
+        <f>CONCATENATE(W$4, "-",$E$125)</f>
+        <v>ro-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="X125" s="52" t="str">
+        <f>CONCATENATE(X$4, "-",$E$125)</f>
+        <v>es-MX-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="Y125" s="52" t="str">
+        <f t="shared" ref="Y125:AQ125" si="2">CONCATENATE(Y$4, "-",$E$125)</f>
+        <v>nb-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="Z125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>bg-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AA125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>hr-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AB125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>et-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AC125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>el-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AD125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>he-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AE125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>hu-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AF125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>lv-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AG125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>lt-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AH125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>pt-BR-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AI125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>sk-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AJ125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>sl-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AK125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>es-AR-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AL125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>th-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AM125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>vi-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AN125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>da-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AO125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>fi-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AP125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>sv-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+      <c r="AQ125" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>tr-As a result of your consent, Philips group companies may contact you with promotional communications via email, SMS and other digital channels, such as mobile apps and social media. To be able to tailor the communications to your preferences and behavior and provide you with the best, personalized experience, we may analyze and combine your personal data. This data may include: \n\nData you give us\nData that you want to actively share with us such as: your name, date of birth or age, email address, physical address, country, gender, phone number, social media profile.\n\nData we get from your interactions with Philips\nData about your interactions and usage of the Philips digital channels, such as social media, websites, emails, apps and connected products. This data may include: IP address, cookies, device information, communications you click on, location details, and websites you visit\n\nPhilips will give you the opportunity to withdraw your consent at any time.\nFor more information, please read the Philips Privacy notice and the Philips Cookie notice.</v>
+      </c>
+    </row>
+    <row r="126" spans="1:43" ht="19" x14ac:dyDescent="0.25">
+      <c r="W126" s="52"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added translation for marketing consent.
</commit_message>
<xml_diff>
--- a/Source/rap/Documents/Internal/Localization/StringLocalization.xlsx
+++ b/Source/rap/Documents/Internal/Localization/StringLocalization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-11940" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-11500" windowWidth="38400" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4558" uniqueCount="3793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4560" uniqueCount="3795">
   <si>
     <t>Reference</t>
   </si>
@@ -34211,13 +34211,19 @@
   </si>
   <si>
     <t>fa-Research and Analytics purpose explanation</t>
+  </si>
+  <si>
+    <t>Marketing consent &amp; what does it mean</t>
+  </si>
+  <si>
+    <t>RA_Setting_Philips_Promo_Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -34351,6 +34357,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial  "/>
     </font>
   </fonts>
   <fills count="5">
@@ -34497,7 +34508,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -34645,6 +34656,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -34924,10 +34936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ124"/>
+  <dimension ref="A1:AQ126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE119" workbookViewId="0">
-      <selection activeCell="AQ124" sqref="AQ124"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49218,7 +49230,7 @@
         <v>3754</v>
       </c>
     </row>
-    <row r="115" spans="1:43" ht="126" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" ht="90" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="50" t="s">
@@ -50823,6 +50835,169 @@
         <f>CONCATENATE(AQ4, "-", E124)</f>
         <v>tr-Research and Analytics purpose explanation</v>
       </c>
+    </row>
+    <row r="125" spans="1:43" ht="38" x14ac:dyDescent="0.25">
+      <c r="C125" s="53" t="s">
+        <v>3794</v>
+      </c>
+      <c r="E125" s="52" t="s">
+        <v>3793</v>
+      </c>
+      <c r="F125" t="str">
+        <f>CONCATENATE(F4, "-", E125)</f>
+        <v>de-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="G125" t="str">
+        <f>CONCATENATE(G4, "-", E125)</f>
+        <v>fr-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="H125" t="str">
+        <f>CONCATENATE(H4, "-", E125)</f>
+        <v>zh-Hans-CN-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="I125" t="str">
+        <f>CONCATENATE(I4, "-", E125)</f>
+        <v>zh-Hant-TW-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="J125" t="str">
+        <f>CONCATENATE(J4, "-", E125)</f>
+        <v>zh-Hant-HK-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="K125" t="str">
+        <f>CONCATENATE(K4, "-", E125)</f>
+        <v>pt-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="L125" t="str">
+        <f>CONCATENATE(L4, "-", E125)</f>
+        <v>ru-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="M125" t="str">
+        <f>CONCATENATE(M4, "-", E125)</f>
+        <v>ar-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="N125" t="str">
+        <f>CONCATENATE(N4, "-", E125)</f>
+        <v>ja-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="O125" t="str">
+        <f>CONCATENATE(O4, "-", E125)</f>
+        <v>nl-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="P125" t="str">
+        <f>CONCATENATE(P4, "-", E125)</f>
+        <v>it-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="Q125" t="str">
+        <f>CONCATENATE(Q4, "-", E125)</f>
+        <v>pl-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="R125" t="str">
+        <f>CONCATENATE(R4, "-", E125)</f>
+        <v>es-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="S125" t="str">
+        <f>CONCATENATE(S4, "-", E125)</f>
+        <v>ko-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="T125" t="str">
+        <f>CONCATENATE(T4, "-", E125)</f>
+        <v>cs-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="U125" t="str">
+        <f>CONCATENATE(U4, "-", E125)</f>
+        <v>en-GB-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="V125" t="str">
+        <f>CONCATENATE(V4, "-", E125)</f>
+        <v>fr-CA-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="W125" t="str">
+        <f>CONCATENATE(W4, "-", E125)</f>
+        <v>ro-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="X125" t="str">
+        <f>CONCATENATE(X4, "-", E125)</f>
+        <v>es-MX-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="Y125" t="str">
+        <f>CONCATENATE(Y4, "-", E125)</f>
+        <v>nb-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="Z125" t="str">
+        <f>CONCATENATE(Z4, "-", E125)</f>
+        <v>bg-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AA125" t="str">
+        <f>CONCATENATE(AA4, "-", E125)</f>
+        <v>hr-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AB125" t="str">
+        <f>CONCATENATE(AB4, "-", E125)</f>
+        <v>et-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AC125" t="str">
+        <f>CONCATENATE(AC4, "-", E125)</f>
+        <v>el-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AD125" t="str">
+        <f>CONCATENATE(AD4, "-", E125)</f>
+        <v>he-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AE125" t="str">
+        <f>CONCATENATE(AE4, "-", E125)</f>
+        <v>hu-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AF125" t="str">
+        <f>CONCATENATE(AF4, "-", E125)</f>
+        <v>lv-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AG125" t="str">
+        <f>CONCATENATE(AG4, "-", E125)</f>
+        <v>lt-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AH125" t="str">
+        <f>CONCATENATE(AH4, "-", E125)</f>
+        <v>pt-BR-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AI125" t="str">
+        <f>CONCATENATE(AI4, "-", E125)</f>
+        <v>sk-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AJ125" t="str">
+        <f>CONCATENATE(AJ4, "-", E125)</f>
+        <v>sl-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AK125" t="str">
+        <f>CONCATENATE(AK4, "-", E125)</f>
+        <v>es-AR-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AL125" t="str">
+        <f>CONCATENATE(AL4, "-", E125)</f>
+        <v>th-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AM125" t="str">
+        <f>CONCATENATE(AM4, "-", E125)</f>
+        <v>vi-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AN125" t="str">
+        <f>CONCATENATE(AN4, "-", E125)</f>
+        <v>da-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AO125" t="str">
+        <f>CONCATENATE(AO4, "-", E125)</f>
+        <v>fi-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AP125" t="str">
+        <f>CONCATENATE(AP4, "-", E125)</f>
+        <v>sv-Marketing consent &amp; what does it mean</v>
+      </c>
+      <c r="AQ125" t="str">
+        <f>CONCATENATE(AQ4, "-", E125)</f>
+        <v>tr-Marketing consent &amp; what does it mean</v>
+      </c>
+    </row>
+    <row r="126" spans="1:43" ht="18" x14ac:dyDescent="0.2">
+      <c r="C126" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>